<commit_message>
adjustment Templating and add API unit test
</commit_message>
<xml_diff>
--- a/Template Mapping Menu AAL.xlsx
+++ b/Template Mapping Menu AAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAL\code-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE9A166-47B3-42F8-AF8B-CB34DEF0EE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330EF651-40CB-41CD-85F4-99E4FADB0328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1AD024CD-D45E-4030-B5EA-57D958362F62}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>MENU NAME</t>
   </si>
@@ -100,40 +100,31 @@
     <t>CTM_NURS_GERM_INVENT</t>
   </si>
   <si>
-    <t>Nursery\Germination</t>
-  </si>
-  <si>
-    <t>CtmNursGermHandling.svc/CtmNursGermSet</t>
-  </si>
-  <si>
-    <t>CtmNursGermInventHandling.svc/CtmNursGermInventSet</t>
-  </si>
-  <si>
-    <t>NursGerm</t>
-  </si>
-  <si>
-    <t>NursGermInvent</t>
-  </si>
-  <si>
     <t>Clone</t>
   </si>
   <si>
-    <t>CtmNurseCloneHandling.svc/CtmNurseCloneSet</t>
-  </si>
-  <si>
     <t>Terima Biji Germination</t>
   </si>
   <si>
     <t>Terima Biji Germination Invent</t>
   </si>
   <si>
-    <t>Nursery\Setup</t>
-  </si>
-  <si>
-    <t>NursClone</t>
-  </si>
-  <si>
     <t>CTM_NURS_CLONE</t>
+  </si>
+  <si>
+    <t>MODULE</t>
+  </si>
+  <si>
+    <t>SUBMODULE</t>
+  </si>
+  <si>
+    <t>Nursery</t>
+  </si>
+  <si>
+    <t>Germination</t>
+  </si>
+  <si>
+    <t>Setup</t>
   </si>
 </sst>
 </file>
@@ -513,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349F67E3-8AEE-43A6-9691-AFCB4D65A015}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,7 +519,7 @@
     <col min="5" max="5" width="48.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,67 +527,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update generator report and navigator registration
</commit_message>
<xml_diff>
--- a/Template Mapping Menu AAL.xlsx
+++ b/Template Mapping Menu AAL.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAL\code-generator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAL\code-generator 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330EF651-40CB-41CD-85F4-99E4FADB0328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1685F-AFC7-43EC-B7C3-BB779956B408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1AD024CD-D45E-4030-B5EA-57D958362F62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1AD024CD-D45E-4030-B5EA-57D958362F62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>MENU NAME</t>
   </si>
@@ -34,66 +34,6 @@
     <t>TABLE NAME</t>
   </si>
   <si>
-    <t>CLASS NAME</t>
-  </si>
-  <si>
-    <t>PACKAGE SUFFIX</t>
-  </si>
-  <si>
-    <t>Master Model</t>
-  </si>
-  <si>
-    <t>CTM_PROD_MODEL</t>
-  </si>
-  <si>
-    <t>ProdModel</t>
-  </si>
-  <si>
-    <t>Service Code</t>
-  </si>
-  <si>
-    <t>CTM_PROD_MODEL_LINE</t>
-  </si>
-  <si>
-    <t>ProdModelLine</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Pf Registration</t>
-  </si>
-  <si>
-    <t>CTM_PF_MAIN_REG</t>
-  </si>
-  <si>
-    <t>PfMainReg</t>
-  </si>
-  <si>
-    <t>COMPANY</t>
-  </si>
-  <si>
-    <t>SITE</t>
-  </si>
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Logistic\Setup</t>
-  </si>
-  <si>
-    <t>Pf\Registration</t>
-  </si>
-  <si>
-    <t>Enterprise\Setup</t>
-  </si>
-  <si>
-    <t>Warranty\Setup</t>
-  </si>
-  <si>
-    <t>IFS PROJECTION</t>
-  </si>
-  <si>
     <t>CTM_NURS_GERM</t>
   </si>
   <si>
@@ -125,6 +65,126 @@
   </si>
   <si>
     <t>Setup</t>
+  </si>
+  <si>
+    <t>ADDL INFO</t>
+  </si>
+  <si>
+    <t>Terima Biji Germination / Detail</t>
+  </si>
+  <si>
+    <t>Terima Biji Pohon Induk</t>
+  </si>
+  <si>
+    <t>Terima Biji Pohon Induk / Detail</t>
+  </si>
+  <si>
+    <t>Overview-Biji per Batch</t>
+  </si>
+  <si>
+    <t>Overview-Biji per Batch / Detail</t>
+  </si>
+  <si>
+    <t>Overview-Biji</t>
+  </si>
+  <si>
+    <t>Penerimaan dan Pengecambahan Biji</t>
+  </si>
+  <si>
+    <t>Penerimaan dan Pengecambahan Biji / Tab 1</t>
+  </si>
+  <si>
+    <t>Penerimaan dan Pengecambahan Biji / Tab 2</t>
+  </si>
+  <si>
+    <t>Penerimaan dan Pengecambahan Biji / Tab 3</t>
+  </si>
+  <si>
+    <t>Cancel Penerimaan dan Pengecambahan Biji</t>
+  </si>
+  <si>
+    <t>Cancel Penerimaan dan Pengecambahan Biji / Tab 1</t>
+  </si>
+  <si>
+    <t>Cancel Penerimaan dan Pengecambahan Biji / Tab 2</t>
+  </si>
+  <si>
+    <t>Cancel Penerimaan dan Pengecambahan Biji / Tab 3</t>
+  </si>
+  <si>
+    <t>Overview-Pengecambahan per Batch</t>
+  </si>
+  <si>
+    <t>Overview-Pengecambahan per Batch / Tab 1</t>
+  </si>
+  <si>
+    <t>Overview Kecambah</t>
+  </si>
+  <si>
+    <t>Pemindahan ke Pre-Nursery</t>
+  </si>
+  <si>
+    <t>Pemindahan ke Pre-Nursery / Tab 1</t>
+  </si>
+  <si>
+    <t>Pemindahan ke Pre-Nursery / Tab 2</t>
+  </si>
+  <si>
+    <t>Cancel Pemindahan ke Pre-Nursery</t>
+  </si>
+  <si>
+    <t>Cancel Pemindahan ke Pre-Nursery / Tab 1</t>
+  </si>
+  <si>
+    <t>Cancel Pemindahan ke Pre-Nursery / Tab 2</t>
+  </si>
+  <si>
+    <t>Overview-Germination Cost History</t>
+  </si>
+  <si>
+    <t>Overview-Germination Transaction History</t>
+  </si>
+  <si>
+    <t>CTM_NURS_GERM_PROCESS</t>
+  </si>
+  <si>
+    <t>CTM_NURS_GERM_TRANS_HIST</t>
+  </si>
+  <si>
+    <t>GERM_GERM_PROCESS_HEADER</t>
+  </si>
+  <si>
+    <t>CTM_NURS_PRE_INVENT</t>
+  </si>
+  <si>
+    <t>CTM_NURS_GERM_COST_HIST</t>
+  </si>
+  <si>
+    <t>Pohon Induk</t>
+  </si>
+  <si>
+    <t>Overview Per Batch</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>RecGer</t>
+  </si>
+  <si>
+    <t>RecGer Tab</t>
+  </si>
+  <si>
+    <t>Cancel RecGer</t>
+  </si>
+  <si>
+    <t>Cancel RecGer Tab</t>
+  </si>
+  <si>
+    <t>Trans Pre Nurs</t>
+  </si>
+  <si>
+    <t>Cancel Trans Pre Nurs</t>
   </si>
 </sst>
 </file>
@@ -156,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -164,32 +224,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,22 +548,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349F67E3-8AEE-43A6-9691-AFCB4D65A015}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,68 +571,460 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{956BE182-0960-4689-93B4-49A906E16E69}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,88 +1043,65 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>